<commit_message>
Some bug-fix for the initial attendance module
</commit_message>
<xml_diff>
--- a/Attendance/test.xlsx
+++ b/Attendance/test.xlsx
@@ -1,3 +1,105 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C34D7D1-45B0-4002-8FC3-98384641ECB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1501" yWindow="0" windowWidth="17558" windowHeight="12464" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="member list" sheetId="1" r:id="rId1"/>
+    <sheet name="05" sheetId="2" r:id="rId2"/>
+  </sheets>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+  <si>
+    <t>Theon</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Attentance days of month</t>
+  </si>
+  <si>
+    <t>Thoen</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -283,26 +385,246 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Theon</t>
-        </is>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>SUM(C2:AG2)</f>
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>